<commit_message>
update member vipdiscountdetail related logic
</commit_message>
<xml_diff>
--- a/AngryCatERP/WebContent/member_sample.xlsx
+++ b/AngryCatERP/WebContent/member_sample.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$5</definedName>
     <definedName name="Gender_Options">Sheet2!$B$2:$B$3</definedName>
     <definedName name="Ohmliy_VIP_Options">Sheet2!$A$2</definedName>
   </definedNames>
@@ -21,16 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>序號</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Ohmliy VIP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Facebook 姓名（中文/英文)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -39,14 +35,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>性別</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>身份證字號</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>電子信箱</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -63,10 +51,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>轉VIP日期</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>備註</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -243,6 +227,30 @@
   </si>
   <si>
     <t>身分證字號為必填；Ohmliy VIP只能填VIP或空白；性別只能填男或女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉VIP起始日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日使用8折優惠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>性別(男或女)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ohmliy VIP(VIP或保持空白)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份證字號(必填)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -309,7 +317,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -326,9 +334,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,238 +631,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="5.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="28.25" customWidth="1"/>
-    <col min="9" max="9" width="23.25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="44.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="28.25" customWidth="1"/>
+    <col min="11" max="11" width="23.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="44.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>24187</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>31872</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="4">
+        <v>36924</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>33028</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4">
+        <v>32459</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
+        <v>35921</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4">
+        <v>24168</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="4">
-        <v>36161</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="4">
-        <v>24187</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="4">
-        <v>36924</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="4">
-        <v>31872</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="4">
-        <v>32459</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="4">
-        <v>33028</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="4">
-        <v>24168</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L5" s="4">
-        <v>35921</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -879,23 +886,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.correct reset function 2.query condition allow hql function 3.MemberVipDiscount add batchVipDate to allow user adjust vip start date 4.check if upload temp dir existed, if not, enforce make one 5.change member upload sample file
</commit_message>
<xml_diff>
--- a/AngryCatERP/WebContent/member_sample.xlsx
+++ b/AngryCatERP/WebContent/member_sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27975" windowHeight="12495"/>
@@ -16,12 +16,12 @@
     <definedName name="Gender_Options">Sheet2!$B$2:$B$3</definedName>
     <definedName name="Ohmliy_VIP_Options">Sheet2!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>序號</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -31,18 +31,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>真實姓名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>電子信箱</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>聯絡電話</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>郵遞區號</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -250,7 +242,49 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>身份證字號(必填)</t>
+    <t>身份證字號</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>真實姓名(必填)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>02-88889999</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>聯絡電話(手機)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>與室內電話擇一必填</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>聯絡電話(室內)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>與手機電話擇一必填</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -258,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +324,14 @@
       <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,7 +359,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -334,6 +376,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,9 +676,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -647,215 +694,233 @@
     <col min="8" max="8" width="16.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.5" style="4" customWidth="1"/>
     <col min="10" max="10" width="28.25" customWidth="1"/>
-    <col min="11" max="11" width="23.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="44.375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="44.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>24187</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42163</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="4">
         <v>36161</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>31872</v>
       </c>
+      <c r="D3" s="4">
+        <v>42248</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I3" s="4">
         <v>36924</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>33028</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42064</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" s="4">
         <v>32459</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>35921</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42248</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" s="4">
         <v>24168</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -886,23 +951,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>